<commit_message>
Implemented hourglass and game start countdown
Added excel of open issues
</commit_message>
<xml_diff>
--- a/PuntiAperti.xlsx
+++ b/PuntiAperti.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>Subject</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>Stesura</t>
+  </si>
+  <si>
+    <t>Chiuso</t>
+  </si>
+  <si>
+    <t>Clessidra</t>
+  </si>
+  <si>
+    <t>Spawn tagli</t>
+  </si>
+  <si>
+    <t>Debug</t>
   </si>
 </sst>
 </file>
@@ -190,14 +202,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:F13" totalsRowCount="1">
-  <autoFilter ref="A1:F12">
-    <filterColumn colId="5"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:F16" totalsRowCount="1">
+  <autoFilter ref="A1:F15"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Subject" totalsRowLabel="Totale"/>
     <tableColumn id="2" name="Issue"/>
-    <tableColumn id="3" name="Effort" totalsRowFunction="sum"/>
+    <tableColumn id="3" name="Effort" totalsRowFunction="custom">
+      <totalsRowFormula>SUM([Effort]) - SUMIF([Status],$D$7,[Effort])</totalsRowFormula>
+    </tableColumn>
     <tableColumn id="4" name="Status"/>
     <tableColumn id="5" name="Facoltativo"/>
     <tableColumn id="6" name="Owner"/>
@@ -491,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
@@ -655,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
@@ -675,13 +687,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -745,12 +757,72 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="C13">
-        <f>SUBTOTAL(109,[Effort])</f>
-        <v>19</v>
+      <c r="C16">
+        <f>SUM([Effort]) - SUMIF([Status],$D$7,[Effort])</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to stage file on open issues :-)
</commit_message>
<xml_diff>
--- a/PuntiAperti.xlsx
+++ b/PuntiAperti.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>Subject</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Debug</t>
+  </si>
+  <si>
+    <t>Marco / Daniele</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,6 +517,7 @@
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -547,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -567,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -607,13 +611,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -627,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -807,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -822,7 +826,7 @@
       </c>
       <c r="C16">
         <f>SUM([Effort]) - SUMIF([Status],$D$7,[Effort])</f>
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>